<commit_message>
bj: add tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Benin/Apr 2023/bj_lf_tas3_202304_3_fts_result.xlsx
+++ b/LF/TAS/Benin/Apr 2023/bj_lf_tas3_202304_3_fts_result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12375" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28125" windowHeight="12375" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
     <t>Ligne témoin discontinue/partielle</t>
   </si>
   <si>
-    <t>Difficulte.d’absorption.d’echantillon</t>
+    <t>Difficulte.d.absorption.d.echantillon</t>
   </si>
   <si>
     <t>Difficulty of absorbing sample</t>
@@ -529,7 +529,7 @@
     <t>Difficulté d’absorption d’échantillon</t>
   </si>
   <si>
-    <t>Difficulte.de.migration.d’echantillon</t>
+    <t>Difficulte.de.migration.d.echantillon</t>
   </si>
   <si>
     <t>Difficulty of migrating sample</t>
@@ -591,12 +591,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -639,18 +639,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -661,9 +654,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -678,22 +670,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -708,10 +707,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -730,16 +737,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -753,6 +752,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -760,15 +767,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -801,187 +810,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,6 +1034,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1036,56 +1054,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1114,6 +1082,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1122,145 +1105,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1362,7 +1377,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1370,46 +1385,48 @@
     <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
     <cellStyle name="Currency" xfId="5" builtinId="4"/>
     <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Check Cell" xfId="8" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="11" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="12" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="13" builtinId="35"/>
-    <cellStyle name="Title" xfId="14" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="15" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="17" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="18" builtinId="19"/>
-    <cellStyle name="Input" xfId="19" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="20" builtinId="40"/>
-    <cellStyle name="Good" xfId="21" builtinId="26"/>
-    <cellStyle name="Output" xfId="22" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="23" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="24" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="25" builtinId="24"/>
-    <cellStyle name="Total" xfId="26" builtinId="25"/>
-    <cellStyle name="Bad" xfId="27" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="29" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="30" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="31" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="33" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="34" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="35" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="37" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="38" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="39" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="40" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="45" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="46" builtinId="52"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -2696,10 +2713,10 @@
   <sheetPr/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="$A4:$XFD5"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -2909,7 +2926,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>